<commit_message>
Optimized python scripts, correct csv and xslx data from Test1
</commit_message>
<xml_diff>
--- a/utils/data/intervalliConfidenza/Test1/CI_Test1_1500ms.xlsx
+++ b/utils/data/intervalliConfidenza/Test1/CI_Test1_1500ms.xlsx
@@ -427,34 +427,34 @@
         <v>11</v>
       </c>
       <c r="B2">
+        <v>53</v>
+      </c>
+      <c r="C2">
         <v>55</v>
-      </c>
-      <c r="C2">
-        <v>53</v>
       </c>
       <c r="D2">
         <v>108</v>
       </c>
       <c r="E2">
-        <v>50.92592592592593</v>
+        <v>49.07407407407408</v>
       </c>
       <c r="F2">
-        <v>6.862072</v>
+        <v>0.330027</v>
       </c>
       <c r="G2">
-        <v>27.689985</v>
+        <v>0.010541</v>
       </c>
       <c r="H2">
-        <v>3.733716815721847</v>
+        <v>0.001447917704583131</v>
       </c>
       <c r="I2">
-        <v>7.31808495881482</v>
+        <v>0.002837918700982937</v>
       </c>
       <c r="J2">
-        <v>14.18015695881482</v>
+        <v>0.3328649187009829</v>
       </c>
       <c r="K2">
-        <v>-0.4560129588148198</v>
+        <v>0.3271890812990171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>